<commit_message>
create a greater clickbus_results to example purpose
</commit_message>
<xml_diff>
--- a/busscraper_input.xlsx
+++ b/busscraper_input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="10">
   <si>
     <t xml:space="preserve">departure_location</t>
   </si>
@@ -56,15 +56,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -124,7 +126,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -134,6 +136,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,13 +160,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.34"/>
   </cols>
@@ -324,6 +330,205 @@
       </c>
       <c r="C13" s="1" t="n">
         <v>45078</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>45079</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>45079</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>45080</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>45080</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>45081</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>45091</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>45081</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>45082</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>45083</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>45085</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>45091</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>45086</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>45087</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>45088</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>45091</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>45089</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>45090</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>45091</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>45091</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>45092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating bugs to accepct return date
</commit_message>
<xml_diff>
--- a/busscraper_input.xlsx
+++ b/busscraper_input.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">departure_date</t>
   </si>
   <si>
-    <t xml:space="preserve">arrival_date</t>
+    <t xml:space="preserve">return_date</t>
   </si>
   <si>
     <t xml:space="preserve">São Paulo</t>
@@ -56,10 +56,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -126,7 +125,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -136,10 +135,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -163,10 +158,10 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.34"/>
   </cols>
@@ -386,7 +381,7 @@
       <c r="C18" s="1" t="n">
         <v>45081</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="1" t="n">
         <v>45091</v>
       </c>
     </row>
@@ -444,7 +439,7 @@
       <c r="C23" s="1" t="n">
         <v>45085</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="1" t="n">
         <v>45091</v>
       </c>
     </row>
@@ -480,7 +475,7 @@
       <c r="C26" s="1" t="n">
         <v>45088</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="1" t="n">
         <v>45091</v>
       </c>
     </row>
@@ -505,7 +500,7 @@
       <c r="C28" s="1" t="n">
         <v>45090</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="D28" s="1" t="n">
         <v>45091</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding debugger to clickbus_scrapper_class & creating buser_scrapper
</commit_message>
<xml_diff>
--- a/busscraper_input.xlsx
+++ b/busscraper_input.xlsx
@@ -56,9 +56,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -125,7 +126,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -134,7 +135,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,13 +168,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.34"/>
   </cols>
@@ -188,47 +201,55 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45084</v>
-      </c>
+        <v>45123</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>45078</v>
-      </c>
+        <v>45108</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>45078</v>
-      </c>
+        <v>45108</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>45084</v>
-      </c>
+        <v>45123</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -238,58 +259,71 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>45078</v>
-      </c>
+        <v>45108</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>45123</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>45084</v>
       </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>45078</v>
-      </c>
+        <v>45108</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>45084</v>
-      </c>
+        <v>45123</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>45078</v>
-      </c>
+        <v>45108</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -299,33 +333,39 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>45084</v>
-      </c>
+        <v>45123</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>45078</v>
-      </c>
+        <v>45108</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>45078</v>
-      </c>
+        <v>45108</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -335,41 +375,49 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>45079</v>
-      </c>
+        <v>45109</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>45079</v>
-      </c>
+        <v>45109</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>45080</v>
-      </c>
+        <v>45110</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>45080</v>
-      </c>
+        <v>45110</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -379,55 +427,65 @@
         <v>7</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>45081</v>
+        <v>45111</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>45091</v>
-      </c>
+        <v>45126</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>45081</v>
-      </c>
+        <v>45111</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>45082</v>
-      </c>
+        <v>45112</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>45083</v>
-      </c>
+        <v>45113</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>45084</v>
-      </c>
+        <v>45114</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -437,33 +495,39 @@
         <v>9</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>45085</v>
+        <v>45115</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>45091</v>
-      </c>
+        <v>45130</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>45086</v>
-      </c>
+        <v>45116</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>45087</v>
-      </c>
+        <v>45117</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -473,22 +537,26 @@
         <v>9</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>45088</v>
+        <v>45118</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>45091</v>
-      </c>
+        <v>45133</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>45089</v>
-      </c>
+        <v>45119</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -498,11 +566,13 @@
         <v>4</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>45090</v>
+        <v>45120</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>45091</v>
       </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -512,19 +582,26 @@
         <v>8</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>45091</v>
-      </c>
+        <v>45121</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>45136</v>
+      </c>
+      <c r="I29" s="4"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>45092</v>
-      </c>
+        <v>45122</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>